<commit_message>
add mock data for last month
</commit_message>
<xml_diff>
--- a/utils/inventory-history.xlsx
+++ b/utils/inventory-history.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayoh\JsProjects\subwai\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D41E516-FC20-45BD-88E6-7AFA94ADC6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D180B70-368A-4978-9226-3DC7B0983F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3DC01F5-3980-4F1C-8323-4E6EC69391B2}"/>
   </bookViews>
@@ -510,7 +510,7 @@
   <dimension ref="A1:AK5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AF12" sqref="AF12"/>
+      <selection activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,9 +620,7 @@
       <c r="AH1" s="1">
         <v>45391</v>
       </c>
-      <c r="AI1" s="1">
-        <v>45398</v>
-      </c>
+      <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
     </row>
@@ -721,16 +719,13 @@
         <v>1.5</v>
       </c>
       <c r="AF2">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="AG2">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AH2">
         <v>0.6</v>
-      </c>
-      <c r="AI2">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
@@ -831,13 +826,10 @@
         <v>0.1</v>
       </c>
       <c r="AG3">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="AH3">
         <v>0.7</v>
-      </c>
-      <c r="AI3">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -935,16 +927,13 @@
         <v>0.25</v>
       </c>
       <c r="AF4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AG4">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="AH4">
-        <v>0.25</v>
-      </c>
-      <c r="AI4">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -1045,13 +1034,10 @@
         <v>0.75</v>
       </c>
       <c r="AG5">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="AH5">
         <v>0.5</v>
-      </c>
-      <c r="AI5">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add better mock data for last month
</commit_message>
<xml_diff>
--- a/utils/inventory-history.xlsx
+++ b/utils/inventory-history.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayoh\JsProjects\subwai\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D180B70-368A-4978-9226-3DC7B0983F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5E86DD-C79D-4B0D-9BBA-12459A690DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3DC01F5-3980-4F1C-8323-4E6EC69391B2}"/>
   </bookViews>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7CDEF5C-ED8E-4292-9935-AABD0103CD70}">
   <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AG7" sqref="AG7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,7 +719,7 @@
         <v>1.5</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="AG2">
         <v>0.75</v>
@@ -820,16 +820,16 @@
         <v>0.1</v>
       </c>
       <c r="AE3">
-        <v>1.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AF3">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="AG3">
         <v>0.8</v>
       </c>
       <c r="AH3">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
@@ -924,16 +924,16 @@
         <v>0.5</v>
       </c>
       <c r="AE4">
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
       <c r="AF4">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="AG4">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AH4">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
@@ -1028,16 +1028,16 @@
         <v>0.5</v>
       </c>
       <c r="AE5">
-        <v>0.625</v>
+        <v>1.3</v>
       </c>
       <c r="AF5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AG5">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="AH5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add better mock data for last week
</commit_message>
<xml_diff>
--- a/utils/inventory-history.xlsx
+++ b/utils/inventory-history.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayoh\JsProjects\subwai\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5E86DD-C79D-4B0D-9BBA-12459A690DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE0688D-7CE5-4F17-A4C8-ED33CF927DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3DC01F5-3980-4F1C-8323-4E6EC69391B2}"/>
   </bookViews>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7CDEF5C-ED8E-4292-9935-AABD0103CD70}">
   <dimension ref="A1:AK5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,16 +1028,16 @@
         <v>0.5</v>
       </c>
       <c r="AE5">
-        <v>1.3</v>
+        <v>0.4</v>
       </c>
       <c r="AF5">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="AG5">
+        <v>0.2</v>
+      </c>
+      <c r="AH5">
         <v>0.8</v>
-      </c>
-      <c r="AH5">
-        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>